<commit_message>
Foi ajustado o erro na parte de edição na classe dermo
</commit_message>
<xml_diff>
--- a/app/data/db_calc_dermo.xlsx
+++ b/app/data/db_calc_dermo.xlsx
@@ -453,17 +453,17 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>1000.0</t>
+          <t>5000.0</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>1000.0</t>
+          <t>5000.0</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>20</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Foi excluído algumas funções não utilizadas
</commit_message>
<xml_diff>
--- a/app/data/db_calc_dermo.xlsx
+++ b/app/data/db_calc_dermo.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -451,19 +451,30 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>5000.0</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>5000.0</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>20</t>
+      <c r="A2" t="n">
+        <v>5000</v>
+      </c>
+      <c r="B2" t="n">
+        <v>5000</v>
+      </c>
+      <c r="C2" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>4000.0</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>4000.0</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>50</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Importações ajustadas, funções do aplicativo testadas com sucesso
</commit_message>
<xml_diff>
--- a/app/data/db_calc_dermo.xlsx
+++ b/app/data/db_calc_dermo.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -450,34 +450,6 @@
         </is>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="n">
-        <v>5000</v>
-      </c>
-      <c r="B2" t="n">
-        <v>5000</v>
-      </c>
-      <c r="C2" t="n">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>4000.0</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>4000.0</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>50</t>
-        </is>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Testes com novos dados
</commit_message>
<xml_diff>
--- a/app/data/db_calc_dermo.xlsx
+++ b/app/data/db_calc_dermo.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -450,6 +450,23 @@
         </is>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>5000.0</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>4000.0</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>